<commit_message>
join all the parsed data from the sheets
</commit_message>
<xml_diff>
--- a/test/assets/simple_data_spreadsheet.xlsx
+++ b/test/assets/simple_data_spreadsheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Contracheque" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,6 +17,7 @@
   <definedNames>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Contracheque!$A$2:$Q$161</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Contracheque!$A$2:$Q$161</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">Contracheque!$A$2:$Q$161</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -367,7 +368,7 @@
     <t xml:space="preserve">Total de Direitos Eventuais</t>
   </si>
   <si>
-    <t xml:space="preserve"> Gratificação Eleitoral </t>
+    <t xml:space="preserve">Gratificação Eleitoral</t>
   </si>
   <si>
     <t xml:space="preserve">fdsa1</t>
@@ -1228,15 +1229,15 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -1256,7 +1257,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -1276,55 +1277,55 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="3" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="8" fillId="4" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="168" fontId="8" fillId="4" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="2" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1332,11 +1333,11 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="4" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="4" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="2" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1380,7 +1381,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -1396,7 +1397,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -1412,11 +1413,11 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1428,7 +1429,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1460,7 +1461,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="170" fontId="0" fillId="0" borderId="25" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -1476,15 +1477,15 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="32" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="33" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1492,11 +1493,11 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="34" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1516,7 +1517,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="25" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -1532,7 +1533,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -1544,23 +1545,23 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="37" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="38" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="39" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="40" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1596,15 +1597,15 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="168" fontId="12" fillId="3" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="42" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1612,15 +1613,15 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="172" fontId="12" fillId="3" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="9" fillId="3" borderId="44" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1652,11 +1653,11 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="14" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="14" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="4" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1679,29 +1680,29 @@
   </sheetPr>
   <dimension ref="A1:X142"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D7" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P21" activeCellId="0" sqref="P21"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H16" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="41.4534412955466"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="41.4534412955466"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="47.3481781376518"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="4" width="19.8178137651822"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="4" width="14.5668016194332"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="4" width="12.4251012145749"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="4" width="15.2105263157895"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="4" width="12.1052631578947"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="4" width="12.6396761133603"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="4" width="13.1740890688259"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="4" width="17.0323886639676"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="4" width="12.6396761133603"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="4" width="12.748987854251"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="4" width="17.7813765182186"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="5" width="12.2105263157895"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="18.5303643724696"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="41.7773279352227"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="41.7773279352227"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="47.7732793522267"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="4" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="4" width="14.6761133603239"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="4" width="12.5344129554656"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="4" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="4" width="12.2105263157895"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="4" width="12.748987854251"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="4" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="4" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="4" width="12.748987854251"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="4" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="4" width="17.8906882591093"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="5" width="12.3198380566802"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="18.6396761133603"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4793,16 +4794,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.5668016194332"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="44.2388663967611"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.6761133603239"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.6396761133603"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.6761133603239"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="44.5627530364373"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.7813765182186"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.748987854251"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.4615384615385"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.9959514170041"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.1052631578947"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.4251012145749"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.1052631578947"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.2105263157895"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.5344129554656"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="48.6315789473684"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="49.0607287449393"/>
     <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -6202,28 +6203,28 @@
   </sheetPr>
   <dimension ref="A1:Q130"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N10" activeCellId="0" sqref="N10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H46" activeCellId="0" sqref="H46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.1417004048583"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="51.0971659919028"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="51.5222672064777"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.9271255060729"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.9595141700405"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.4615384615385"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.6396761133603"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.0688259109312"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.5668016194332"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.748987854251"/>
     <col collapsed="false" hidden="false" max="8" min="7" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.5344129554656"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.6396761133603"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="13.0688259109312"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.9271255060729"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.6761133603239"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="12.4251012145749"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="12.2105263157895"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="14.5668016194332"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="12.5344129554656"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="12.3198380566802"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="14.6761133603239"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="42.4210526315789"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="42.7408906882591"/>
     <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -8692,7 +8693,7 @@
       <c r="N128" s="79"/>
       <c r="O128" s="78"/>
     </row>
-    <row r="129" s="45" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="42"/>
       <c r="B129" s="0"/>
       <c r="C129" s="78"/>
@@ -8755,31 +8756,31 @@
   </sheetPr>
   <dimension ref="A1:S130"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P9" activeCellId="0" sqref="P9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M16" activeCellId="0" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.0323886639676"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="51.0971659919028"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="51.5222672064777"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.2834008097166"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.3562753036437"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.1052631578947"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.9959514170041"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.4251012145749"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.0688259109312"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="15.5303643724696"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.2105263157895"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.1052631578947"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.5344129554656"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="15.6396761133603"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.6761133603239"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="12.4251012145749"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="12.2105263157895"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="12.4251012145749"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="12.5344129554656"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="12.3198380566802"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="12.5344129554656"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="17" min="17" style="0" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="18" min="18" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="50.8825910931174"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="51.3117408906883"/>
     <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -8926,7 +8927,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="38" t="str">
         <f aca="false">'Dados Cadastrais'!A5</f>
         <v>xxx.xxx.xxx-xx</v>
@@ -8982,7 +8983,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="38" t="str">
         <f aca="false">'Dados Cadastrais'!A6</f>
         <v>xxx.xxx.xxx-xx</v>
@@ -9038,7 +9039,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="38" t="str">
         <f aca="false">'Dados Cadastrais'!A7</f>
         <v>xxx.xxx.xxx-xx</v>
@@ -9094,7 +9095,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="38" t="str">
         <f aca="false">'Dados Cadastrais'!A8</f>
         <v>xxx.xxx.xxx-xx</v>
@@ -11415,7 +11416,7 @@
       <c r="P128" s="79"/>
       <c r="Q128" s="78"/>
     </row>
-    <row r="129" s="45" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="42"/>
       <c r="B129" s="0"/>
       <c r="C129" s="78"/>
@@ -11488,14 +11489,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="91" width="14.5668016194332"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.2753036437247"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.2105263157895"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="37.7044534412955"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="46.2753036437247"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.7813765182186"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="37.17004048583"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="91" width="14.6761133603239"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.5951417004049"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="37.919028340081"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="46.5951417004049"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.995951417004"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="37.4898785425101"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.6032388663968"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>

</xml_diff>